<commit_message>
added few extra results into excel
</commit_message>
<xml_diff>
--- a/Data regarding CNN testing.xlsx
+++ b/Data regarding CNN testing.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\phuoc\OneDrive\Desktop\School\ML Boot Camp\Projects\Project_3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70341A78-5D07-473C-B4A2-B17AD9A636AA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{587B8BCE-C1B6-4C3C-95BD-E74F08AF9472}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4404" yWindow="1032" windowWidth="17280" windowHeight="8964" xr2:uid="{B810E98E-C342-446B-AE56-9010DD8D8D6E}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Convolutions</t>
   </si>
@@ -63,6 +63,9 @@
   </si>
   <si>
     <t>I saw the loss value increase at 3, so I wanted to test and see if we get a better result this way</t>
+  </si>
+  <si>
+    <t>Random testing</t>
   </si>
 </sst>
 </file>
@@ -96,7 +99,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -260,6 +263,54 @@
       </right>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -267,7 +318,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -290,6 +341,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -605,10 +662,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{552E8CC1-DEB4-4FE5-B22D-00FDC7A64A7D}">
-  <dimension ref="B2:H12"/>
+  <dimension ref="B2:H14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -770,6 +827,9 @@
       <c r="F9" s="18">
         <v>0.84921999999999997</v>
       </c>
+      <c r="H9" s="25" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B10" s="13">
@@ -787,46 +847,84 @@
       <c r="F10" s="15">
         <v>0.85918000000000005</v>
       </c>
-    </row>
-    <row r="11" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="19">
+      <c r="H10" s="26"/>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B11" s="13">
         <v>2</v>
       </c>
-      <c r="C11" s="20">
+      <c r="C11" s="14">
         <v>250</v>
       </c>
-      <c r="D11" s="20">
+      <c r="D11" s="14">
         <v>3</v>
       </c>
-      <c r="E11" s="20">
+      <c r="E11" s="14">
         <v>229</v>
       </c>
-      <c r="F11" s="21">
+      <c r="F11" s="15">
         <v>0.79005999999999998</v>
       </c>
-      <c r="H11" t="s">
+      <c r="H11" s="27" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="3">
+    <row r="12" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B12" s="23">
         <v>2</v>
       </c>
-      <c r="C12" s="4">
+      <c r="C12" s="22">
         <v>200</v>
       </c>
-      <c r="D12" s="4">
+      <c r="D12" s="22">
         <v>3</v>
       </c>
-      <c r="E12" s="4">
+      <c r="E12" s="22">
         <v>207</v>
       </c>
-      <c r="F12" s="21">
+      <c r="F12" s="24">
         <v>0.86072300000000002</v>
       </c>
+      <c r="H12" s="26"/>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B13" s="13">
+        <v>3</v>
+      </c>
+      <c r="C13" s="14">
+        <v>250</v>
+      </c>
+      <c r="D13" s="14">
+        <v>5</v>
+      </c>
+      <c r="E13" s="14">
+        <v>220</v>
+      </c>
+      <c r="F13" s="15">
+        <v>0.89081999999999995</v>
+      </c>
+      <c r="H13" s="26"/>
+    </row>
+    <row r="14" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B14" s="19">
+        <v>3</v>
+      </c>
+      <c r="C14" s="20">
+        <v>250</v>
+      </c>
+      <c r="D14" s="20">
+        <v>3</v>
+      </c>
+      <c r="E14" s="20">
+        <v>220</v>
+      </c>
+      <c r="F14" s="21">
+        <v>0.86873999999999996</v>
+      </c>
+      <c r="H14" s="7"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="F3:F12">
+  <conditionalFormatting sqref="F3:F14">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>